<commit_message>
Changed file name formatting of example data
</commit_message>
<xml_diff>
--- a/example_data/FarmToFork_Invoice_Contacts.xlsx
+++ b/example_data/FarmToFork_Invoice_Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbrierley/Code/F2F/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB35686-AD98-B143-9E51-DDE51AE59302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38906BFF-9DCC-334F-9AE9-F46A55FF68F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8F378BB0-B83A-A44D-8EFE-3CC700C1BBAE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>Balliol</t>
   </si>
@@ -219,13 +219,70 @@
   </si>
   <si>
     <t>St Anne's</t>
+  </si>
+  <si>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>F2F456</t>
+  </si>
+  <si>
+    <t>F2F457</t>
+  </si>
+  <si>
+    <t>F2F458</t>
+  </si>
+  <si>
+    <t>F2F459</t>
+  </si>
+  <si>
+    <t>F2F460</t>
+  </si>
+  <si>
+    <t>F2F461</t>
+  </si>
+  <si>
+    <t>F2F462</t>
+  </si>
+  <si>
+    <t>F2F463</t>
+  </si>
+  <si>
+    <t>F2F464</t>
+  </si>
+  <si>
+    <t>F2F465</t>
+  </si>
+  <si>
+    <t>F2F466</t>
+  </si>
+  <si>
+    <t>F2F467</t>
+  </si>
+  <si>
+    <t>F2F468</t>
+  </si>
+  <si>
+    <t>F2F469</t>
+  </si>
+  <si>
+    <t>F2F470</t>
+  </si>
+  <si>
+    <t>F2F471</t>
+  </si>
+  <si>
+    <t>F2F472</t>
+  </si>
+  <si>
+    <t>F2F473</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +295,13 @@
       <color rgb="FF202124"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,9 +324,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66AE39D3-A9D3-124B-A0F9-8AE5C0919E49}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,12 +656,12 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="36.33203125" customWidth="1"/>
     <col min="9" max="9" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -615,8 +680,11 @@
       <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,8 +699,11 @@
         <v>20</v>
       </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -647,8 +718,11 @@
         <v>21</v>
       </c>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -663,8 +737,11 @@
         <v>22</v>
       </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -679,8 +756,11 @@
         <v>23</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -695,8 +775,11 @@
         <v>24</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -711,8 +794,11 @@
         <v>25</v>
       </c>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -727,8 +813,11 @@
         <v>26</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -743,8 +832,11 @@
         <v>27</v>
       </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -759,8 +851,11 @@
         <v>28</v>
       </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -775,8 +870,11 @@
         <v>29</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -791,8 +889,11 @@
         <v>30</v>
       </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -807,8 +908,11 @@
         <v>31</v>
       </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -823,8 +927,11 @@
         <v>32</v>
       </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -839,8 +946,11 @@
         <v>33</v>
       </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -855,8 +965,11 @@
         <v>34</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -871,8 +984,11 @@
         <v>35</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -887,8 +1003,11 @@
         <v>36</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -903,6 +1022,9 @@
         <v>37</v>
       </c>
       <c r="F19" s="1"/>
+      <c r="G19" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added VAT tab on contacts
</commit_message>
<xml_diff>
--- a/example_data/FarmToFork_Invoice_Contacts.xlsx
+++ b/example_data/FarmToFork_Invoice_Contacts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbrierley/Code/F2F/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29F342A-C467-9D40-833F-C630CCBABAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8AD0BB-59E5-F342-8B9A-EC32E7C23BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8F378BB0-B83A-A44D-8EFE-3CC700C1BBAE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{8F378BB0-B83A-A44D-8EFE-3CC700C1BBAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="VAT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>Balliol</t>
   </si>
@@ -279,6 +280,51 @@
   </si>
   <si>
     <t>St Catherine’s</t>
+  </si>
+  <si>
+    <t>Seller</t>
+  </si>
+  <si>
+    <t>VAT Y/N?</t>
+  </si>
+  <si>
+    <t>Blacklands</t>
+  </si>
+  <si>
+    <t>Worthy Earth at Bletchingdon</t>
+  </si>
+  <si>
+    <t>Bruern Farms</t>
+  </si>
+  <si>
+    <t>Nettlebed Creamery</t>
+  </si>
+  <si>
+    <t>Oxford City Farm</t>
+  </si>
+  <si>
+    <t>Rose Dale’s Organic Farm</t>
+  </si>
+  <si>
+    <t>Sandy Lane Organics</t>
+  </si>
+  <si>
+    <t>Willowbrook Farm</t>
+  </si>
+  <si>
+    <t>Forge Farm</t>
+  </si>
+  <si>
+    <t>Brighthampton Veg</t>
+  </si>
+  <si>
+    <t>Pudlicote Farm</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -647,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66AE39D3-A9D3-124B-A0F9-8AE5C0919E49}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1038,4 +1084,131 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3335A2FA-C3DC-4547-BEE2-E981CAC53876}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.facebook.com/BlacklandsOrganics/?locale=en_GB" xr:uid="{8B5F5978-D469-F347-ACDF-50DD24FD7AB0}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://worthy-earth.co.uk/" xr:uid="{F3467C97-3966-F54E-B885-09494A4C84B3}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://bruernfarms.co.uk/" xr:uid="{BB6BE909-A415-3C47-9739-3FDBD7B2185E}"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://www.nettlebedcreamery.com/" xr:uid="{3D6FC9C2-26A3-484F-95C7-3E11C8F13A43}"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://www.oxfordcityfarm.org.uk/" xr:uid="{ECF27178-01B7-C145-A860-95A5A633A6A7}"/>
+    <hyperlink ref="A7" r:id="rId6" display="http://ww.rosedalesorganicfarm.com/" xr:uid="{F28C29A4-5FB2-EA42-9326-1CEC169BDB5E}"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://sandylanefarm.co.uk/" xr:uid="{5BBC9DD0-DA9D-FC46-93DD-EEE75885B10E}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.willowbrookfarm.co.uk/" xr:uid="{317B0FA6-19CE-4549-81AF-392155336DB1}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.forgefarm.com/" xr:uid="{378BF59F-3E99-8B4B-B93D-5335D3142262}"/>
+    <hyperlink ref="A12" r:id="rId10" display="www.pudlicotefarm.co.uk" xr:uid="{B8ECCACB-1EC7-8C41-9F0B-2213F918F3F1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added buyer full name column
</commit_message>
<xml_diff>
--- a/example_data/FarmToFork_Invoice_Contacts.xlsx
+++ b/example_data/FarmToFork_Invoice_Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbrierley/Code/F2F/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FD7EF0-5D76-9C4F-81B8-310992B0064D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E59A6F-F442-5B46-891E-E5F82691BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8F378BB0-B83A-A44D-8EFE-3CC700C1BBAE}"/>
   </bookViews>
@@ -293,9 +293,6 @@
     <t>Jesus College</t>
   </si>
   <si>
-    <t>Lady Margarate Hall</t>
-  </si>
-  <si>
     <t>Linacre College</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>Buyer Key as in Spreadsheet</t>
+  </si>
+  <si>
+    <t>Lady Margaret Hall</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66AE39D3-A9D3-124B-A0F9-8AE5C0919E49}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -715,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>80</v>
@@ -854,7 +856,7 @@
         <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>51</v>
@@ -876,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>38</v>
@@ -898,7 +900,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -920,7 +922,7 @@
         <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
@@ -942,7 +944,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>41</v>
@@ -964,7 +966,7 @@
         <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
@@ -986,7 +988,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>43</v>
@@ -1008,7 +1010,7 @@
         <v>79</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>44</v>
@@ -1052,7 +1054,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>46</v>
@@ -1074,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
@@ -1096,7 +1098,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>47</v>
@@ -1118,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Added automatic invoice and order numbers
</commit_message>
<xml_diff>
--- a/example_data/FarmToFork_Invoice_Contacts.xlsx
+++ b/example_data/FarmToFork_Invoice_Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbrierley/Code/F2F/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E59A6F-F442-5B46-891E-E5F82691BAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEE79B7-B440-BE46-BA07-4F2427145AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8F378BB0-B83A-A44D-8EFE-3CC700C1BBAE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
   <si>
     <t>Balliol</t>
   </si>
@@ -204,63 +204,6 @@
   </si>
   <si>
     <t>St Anne's</t>
-  </si>
-  <si>
-    <t>Invoice Number</t>
-  </si>
-  <si>
-    <t>F2F456</t>
-  </si>
-  <si>
-    <t>F2F457</t>
-  </si>
-  <si>
-    <t>F2F458</t>
-  </si>
-  <si>
-    <t>F2F459</t>
-  </si>
-  <si>
-    <t>F2F460</t>
-  </si>
-  <si>
-    <t>F2F461</t>
-  </si>
-  <si>
-    <t>F2F462</t>
-  </si>
-  <si>
-    <t>F2F463</t>
-  </si>
-  <si>
-    <t>F2F464</t>
-  </si>
-  <si>
-    <t>F2F465</t>
-  </si>
-  <si>
-    <t>F2F466</t>
-  </si>
-  <si>
-    <t>F2F467</t>
-  </si>
-  <si>
-    <t>F2F468</t>
-  </si>
-  <si>
-    <t>F2F469</t>
-  </si>
-  <si>
-    <t>F2F470</t>
-  </si>
-  <si>
-    <t>F2F471</t>
-  </si>
-  <si>
-    <t>F2F472</t>
-  </si>
-  <si>
-    <t>F2F473</t>
   </si>
   <si>
     <t>LMH</t>
@@ -699,7 +642,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,10 +660,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -737,16 +680,14 @@
       <c r="G1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -759,9 +700,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -781,16 +720,14 @@
         <v>16</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>50</v>
@@ -803,16 +740,14 @@
         <v>17</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>36</v>
@@ -825,16 +760,14 @@
         <v>18</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>37</v>
@@ -847,16 +780,14 @@
         <v>19</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>51</v>
@@ -869,16 +800,14 @@
         <v>20</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>38</v>
@@ -891,16 +820,14 @@
         <v>21</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -913,16 +840,14 @@
         <v>22</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
@@ -935,16 +860,14 @@
         <v>23</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>41</v>
@@ -957,16 +880,14 @@
         <v>24</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
@@ -979,16 +900,14 @@
         <v>25</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>43</v>
@@ -1001,16 +920,14 @@
         <v>26</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>44</v>
@@ -1023,16 +940,14 @@
         <v>27</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>45</v>
@@ -1045,16 +960,14 @@
         <v>28</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>46</v>
@@ -1067,16 +980,14 @@
         <v>29</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
@@ -1089,16 +1000,14 @@
         <v>30</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>47</v>
@@ -1111,16 +1020,14 @@
         <v>31</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>48</v>
@@ -1133,13 +1040,11 @@
         <v>32</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="H19" s="2"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P28" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>